<commit_message>
Topics addition for programme
</commit_message>
<xml_diff>
--- a/DataScience_Project.xlsx
+++ b/DataScience_Project.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\30158\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\30158\Desktop\P-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Dev Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Topics" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Project Data Science</t>
   </si>
@@ -96,6 +97,33 @@
   </si>
   <si>
     <t>Data Collection, Project Repository Creation</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Topics</t>
+  </si>
+  <si>
+    <t>Probability Theorems</t>
+  </si>
+  <si>
+    <t>Hypothesis Testing</t>
+  </si>
+  <si>
+    <t>Probalility Distribution</t>
+  </si>
+  <si>
+    <t>Mathmatical Modeling of Linear Progammes</t>
+  </si>
+  <si>
+    <t>Mathematical Modeling of Integer Programmes</t>
+  </si>
+  <si>
+    <t>One-to-One allocation problem optimisation</t>
+  </si>
+  <si>
+    <t>Using Excel Solver for Analysis</t>
   </si>
 </sst>
 </file>
@@ -126,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +179,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -164,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -174,6 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -599,4 +634,72 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>